<commit_message>
ADD: LLM train dataset (fin)
</commit_message>
<xml_diff>
--- a/2025_05_02_OhLoRA_v2/llm/fine_tuning_dataset/OhLoRA_fine_tuning_v2.xlsx
+++ b/2025_05_02_OhLoRA_v2/llm/fine_tuning_dataset/OhLoRA_fine_tuning_v2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A68574C3-20A6-4724-86DB-0FD76AD4F495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2DB7E871-DB4E-403B-9BCD-DC94B9B7E1A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18816" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3204" uniqueCount="1361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3510" uniqueCount="1361">
   <si>
     <t>data_type</t>
   </si>
@@ -8394,12 +8394,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I527"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A301" workbookViewId="0">
+      <selection activeCell="C375" sqref="C375"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="67.796875" customWidth="1"/>
-    <col min="3" max="3" width="65.296875" customWidth="1"/>
+    <col min="2" max="2" width="32.8984375" customWidth="1"/>
+    <col min="3" max="3" width="43.3984375" customWidth="1"/>
     <col min="4" max="4" width="26.296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="39.296875" customWidth="1"/>
     <col min="6" max="6" width="35.19921875" customWidth="1"/>
@@ -18379,7 +18381,16 @@
       </c>
       <c r="F356" t="str">
         <f t="shared" si="5"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
+        <v>(눈 보통, 입 크게, 고개 돌림 없음)</v>
+      </c>
+      <c r="G356" t="s">
+        <v>988</v>
+      </c>
+      <c r="H356" t="s">
+        <v>991</v>
+      </c>
+      <c r="I356" t="s">
+        <v>990</v>
       </c>
     </row>
     <row r="357" spans="1:9" x14ac:dyDescent="0.4">
@@ -18397,7 +18408,16 @@
       </c>
       <c r="F357" t="str">
         <f t="shared" ref="F357:F420" si="6">"(눈 "&amp;G357&amp;", 입 "&amp;H357&amp;", 고개 돌림 "&amp;I357&amp;")"</f>
-        <v>(눈 , 입 , 고개 돌림 )</v>
+        <v>(눈 보통, 입 크게, 고개 돌림 없음)</v>
+      </c>
+      <c r="G357" t="s">
+        <v>988</v>
+      </c>
+      <c r="H357" t="s">
+        <v>991</v>
+      </c>
+      <c r="I357" t="s">
+        <v>990</v>
       </c>
     </row>
     <row r="358" spans="1:9" x14ac:dyDescent="0.4">
@@ -18415,7 +18435,16 @@
       </c>
       <c r="F358" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
+        <v>(눈 보통, 입 크게, 고개 돌림 없음)</v>
+      </c>
+      <c r="G358" t="s">
+        <v>988</v>
+      </c>
+      <c r="H358" t="s">
+        <v>991</v>
+      </c>
+      <c r="I358" t="s">
+        <v>990</v>
       </c>
     </row>
     <row r="359" spans="1:9" x14ac:dyDescent="0.4">
@@ -18433,7 +18462,16 @@
       </c>
       <c r="F359" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
+        <v>(눈 보통, 입 크게, 고개 돌림 없음)</v>
+      </c>
+      <c r="G359" t="s">
+        <v>988</v>
+      </c>
+      <c r="H359" t="s">
+        <v>991</v>
+      </c>
+      <c r="I359" t="s">
+        <v>990</v>
       </c>
     </row>
     <row r="360" spans="1:9" x14ac:dyDescent="0.4">
@@ -18451,7 +18489,16 @@
       </c>
       <c r="F360" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
+        <v>(눈 보통, 입 크게, 고개 돌림 없음)</v>
+      </c>
+      <c r="G360" t="s">
+        <v>988</v>
+      </c>
+      <c r="H360" t="s">
+        <v>991</v>
+      </c>
+      <c r="I360" t="s">
+        <v>990</v>
       </c>
     </row>
     <row r="361" spans="1:9" x14ac:dyDescent="0.4">
@@ -18469,7 +18516,16 @@
       </c>
       <c r="F361" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
+        <v>(눈 보통, 입 크게, 고개 돌림 없음)</v>
+      </c>
+      <c r="G361" t="s">
+        <v>988</v>
+      </c>
+      <c r="H361" t="s">
+        <v>991</v>
+      </c>
+      <c r="I361" t="s">
+        <v>990</v>
       </c>
     </row>
     <row r="362" spans="1:9" x14ac:dyDescent="0.4">
@@ -18487,7 +18543,16 @@
       </c>
       <c r="F362" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
+        <v>(눈 보통, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G362" t="s">
+        <v>988</v>
+      </c>
+      <c r="H362" t="s">
+        <v>988</v>
+      </c>
+      <c r="I362" t="s">
+        <v>990</v>
       </c>
     </row>
     <row r="363" spans="1:9" x14ac:dyDescent="0.4">
@@ -18505,7 +18570,16 @@
       </c>
       <c r="F363" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
+        <v>(눈 보통, 입 크게, 고개 돌림 없음)</v>
+      </c>
+      <c r="G363" t="s">
+        <v>988</v>
+      </c>
+      <c r="H363" t="s">
+        <v>991</v>
+      </c>
+      <c r="I363" t="s">
+        <v>990</v>
       </c>
     </row>
     <row r="364" spans="1:9" x14ac:dyDescent="0.4">
@@ -18523,7 +18597,16 @@
       </c>
       <c r="F364" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
+        <v>(눈 크게, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G364" t="s">
+        <v>991</v>
+      </c>
+      <c r="H364" t="s">
+        <v>988</v>
+      </c>
+      <c r="I364" t="s">
+        <v>990</v>
       </c>
     </row>
     <row r="365" spans="1:9" x14ac:dyDescent="0.4">
@@ -18541,7 +18624,16 @@
       </c>
       <c r="F365" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
+        <v>(눈 보통, 입 크게, 고개 돌림 없음)</v>
+      </c>
+      <c r="G365" t="s">
+        <v>988</v>
+      </c>
+      <c r="H365" t="s">
+        <v>991</v>
+      </c>
+      <c r="I365" t="s">
+        <v>990</v>
       </c>
     </row>
     <row r="366" spans="1:9" x14ac:dyDescent="0.4">
@@ -18559,7 +18651,16 @@
       </c>
       <c r="F366" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
+        <v>(눈 크게, 입 크게, 고개 돌림 없음)</v>
+      </c>
+      <c r="G366" t="s">
+        <v>991</v>
+      </c>
+      <c r="H366" t="s">
+        <v>991</v>
+      </c>
+      <c r="I366" t="s">
+        <v>990</v>
       </c>
     </row>
     <row r="367" spans="1:9" x14ac:dyDescent="0.4">
@@ -18577,7 +18678,16 @@
       </c>
       <c r="F367" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
+        <v>(눈 크게, 입 크게, 고개 돌림 없음)</v>
+      </c>
+      <c r="G367" t="s">
+        <v>991</v>
+      </c>
+      <c r="H367" t="s">
+        <v>991</v>
+      </c>
+      <c r="I367" t="s">
+        <v>990</v>
       </c>
     </row>
     <row r="368" spans="1:9" x14ac:dyDescent="0.4">
@@ -18598,10 +18708,19 @@
       </c>
       <c r="F368" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="369" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 보통, 입 크게, 고개 돌림 없음)</v>
+      </c>
+      <c r="G368" t="s">
+        <v>988</v>
+      </c>
+      <c r="H368" t="s">
+        <v>991</v>
+      </c>
+      <c r="I368" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="369" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A369" t="s">
         <v>4</v>
       </c>
@@ -18616,10 +18735,19 @@
       </c>
       <c r="F369" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="370" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 보통, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G369" t="s">
+        <v>988</v>
+      </c>
+      <c r="H369" t="s">
+        <v>988</v>
+      </c>
+      <c r="I369" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="370" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A370" t="s">
         <v>4</v>
       </c>
@@ -18634,10 +18762,19 @@
       </c>
       <c r="F370" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="371" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 크게, 입 크게, 고개 돌림 없음)</v>
+      </c>
+      <c r="G370" t="s">
+        <v>991</v>
+      </c>
+      <c r="H370" t="s">
+        <v>991</v>
+      </c>
+      <c r="I370" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="371" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A371" t="s">
         <v>4</v>
       </c>
@@ -18655,10 +18792,19 @@
       </c>
       <c r="F371" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="372" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 크게, 입 아주 크게, 고개 돌림 없음)</v>
+      </c>
+      <c r="G371" t="s">
+        <v>991</v>
+      </c>
+      <c r="H371" t="s">
+        <v>992</v>
+      </c>
+      <c r="I371" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="372" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A372" t="s">
         <v>4</v>
       </c>
@@ -18673,10 +18819,19 @@
       </c>
       <c r="F372" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="373" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 보통, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G372" t="s">
+        <v>988</v>
+      </c>
+      <c r="H372" t="s">
+        <v>988</v>
+      </c>
+      <c r="I372" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="373" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A373" t="s">
         <v>4</v>
       </c>
@@ -18694,10 +18849,19 @@
       </c>
       <c r="F373" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="374" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 보통, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G373" t="s">
+        <v>988</v>
+      </c>
+      <c r="H373" t="s">
+        <v>988</v>
+      </c>
+      <c r="I373" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="374" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A374" t="s">
         <v>4</v>
       </c>
@@ -18715,10 +18879,19 @@
       </c>
       <c r="F374" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="375" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 아주 크게, 입 아주 크게, 고개 돌림 없음)</v>
+      </c>
+      <c r="G374" t="s">
+        <v>992</v>
+      </c>
+      <c r="H374" t="s">
+        <v>992</v>
+      </c>
+      <c r="I374" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="375" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A375" t="s">
         <v>4</v>
       </c>
@@ -18733,10 +18906,19 @@
       </c>
       <c r="F375" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="376" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 작게, 입 보통, 고개 돌림 보통)</v>
+      </c>
+      <c r="G375" t="s">
+        <v>987</v>
+      </c>
+      <c r="H375" t="s">
+        <v>988</v>
+      </c>
+      <c r="I375" t="s">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="376" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A376" t="s">
         <v>4</v>
       </c>
@@ -18751,10 +18933,19 @@
       </c>
       <c r="F376" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="377" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 크게, 입 크게, 고개 돌림 없음)</v>
+      </c>
+      <c r="G376" t="s">
+        <v>991</v>
+      </c>
+      <c r="H376" t="s">
+        <v>991</v>
+      </c>
+      <c r="I376" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="377" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A377" t="s">
         <v>4</v>
       </c>
@@ -18769,10 +18960,19 @@
       </c>
       <c r="F377" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="378" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 보통, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G377" t="s">
+        <v>988</v>
+      </c>
+      <c r="H377" t="s">
+        <v>988</v>
+      </c>
+      <c r="I377" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="378" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A378" t="s">
         <v>4</v>
       </c>
@@ -18790,10 +18990,19 @@
       </c>
       <c r="F378" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="379" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 보통, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G378" t="s">
+        <v>988</v>
+      </c>
+      <c r="H378" t="s">
+        <v>988</v>
+      </c>
+      <c r="I378" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="379" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A379" t="s">
         <v>4</v>
       </c>
@@ -18811,10 +19020,19 @@
       </c>
       <c r="F379" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="380" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 보통, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G379" t="s">
+        <v>988</v>
+      </c>
+      <c r="H379" t="s">
+        <v>988</v>
+      </c>
+      <c r="I379" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="380" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A380" t="s">
         <v>4</v>
       </c>
@@ -18829,10 +19047,19 @@
       </c>
       <c r="F380" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="381" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 보통, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G380" t="s">
+        <v>988</v>
+      </c>
+      <c r="H380" t="s">
+        <v>988</v>
+      </c>
+      <c r="I380" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="381" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A381" t="s">
         <v>4</v>
       </c>
@@ -18847,10 +19074,19 @@
       </c>
       <c r="F381" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="382" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 보통, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G381" t="s">
+        <v>988</v>
+      </c>
+      <c r="H381" t="s">
+        <v>988</v>
+      </c>
+      <c r="I381" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="382" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A382" t="s">
         <v>4</v>
       </c>
@@ -18865,10 +19101,19 @@
       </c>
       <c r="F382" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="383" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 보통, 입 크게, 고개 돌림 없음)</v>
+      </c>
+      <c r="G382" t="s">
+        <v>988</v>
+      </c>
+      <c r="H382" t="s">
+        <v>991</v>
+      </c>
+      <c r="I382" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="383" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A383" t="s">
         <v>4</v>
       </c>
@@ -18886,10 +19131,19 @@
       </c>
       <c r="F383" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="384" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 보통, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G383" t="s">
+        <v>988</v>
+      </c>
+      <c r="H383" t="s">
+        <v>988</v>
+      </c>
+      <c r="I383" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="384" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A384" t="s">
         <v>4</v>
       </c>
@@ -18904,10 +19158,19 @@
       </c>
       <c r="F384" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="385" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 보통, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G384" t="s">
+        <v>988</v>
+      </c>
+      <c r="H384" t="s">
+        <v>988</v>
+      </c>
+      <c r="I384" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="385" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A385" t="s">
         <v>4</v>
       </c>
@@ -18922,10 +19185,19 @@
       </c>
       <c r="F385" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="386" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 보통, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G385" t="s">
+        <v>988</v>
+      </c>
+      <c r="H385" t="s">
+        <v>988</v>
+      </c>
+      <c r="I385" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="386" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A386" t="s">
         <v>4</v>
       </c>
@@ -18943,10 +19215,19 @@
       </c>
       <c r="F386" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="387" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 크게, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G386" t="s">
+        <v>991</v>
+      </c>
+      <c r="H386" t="s">
+        <v>988</v>
+      </c>
+      <c r="I386" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="387" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A387" t="s">
         <v>4</v>
       </c>
@@ -18961,10 +19242,19 @@
       </c>
       <c r="F387" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="388" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 보통, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G387" t="s">
+        <v>988</v>
+      </c>
+      <c r="H387" t="s">
+        <v>988</v>
+      </c>
+      <c r="I387" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="388" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A388" t="s">
         <v>4</v>
       </c>
@@ -18979,10 +19269,19 @@
       </c>
       <c r="F388" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="389" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 보통, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G388" t="s">
+        <v>988</v>
+      </c>
+      <c r="H388" t="s">
+        <v>988</v>
+      </c>
+      <c r="I388" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="389" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A389" t="s">
         <v>4</v>
       </c>
@@ -19000,10 +19299,19 @@
       </c>
       <c r="F389" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="390" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 보통, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G389" t="s">
+        <v>988</v>
+      </c>
+      <c r="H389" t="s">
+        <v>988</v>
+      </c>
+      <c r="I389" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="390" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A390" t="s">
         <v>4</v>
       </c>
@@ -19018,10 +19326,19 @@
       </c>
       <c r="F390" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="391" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 보통, 입 크게, 고개 돌림 없음)</v>
+      </c>
+      <c r="G390" t="s">
+        <v>988</v>
+      </c>
+      <c r="H390" t="s">
+        <v>991</v>
+      </c>
+      <c r="I390" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="391" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A391" t="s">
         <v>4</v>
       </c>
@@ -19036,10 +19353,19 @@
       </c>
       <c r="F391" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="392" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 크게, 입 크게, 고개 돌림 없음)</v>
+      </c>
+      <c r="G391" t="s">
+        <v>991</v>
+      </c>
+      <c r="H391" t="s">
+        <v>991</v>
+      </c>
+      <c r="I391" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="392" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A392" t="s">
         <v>4</v>
       </c>
@@ -19054,10 +19380,19 @@
       </c>
       <c r="F392" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="393" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 보통, 입 보통, 고개 돌림 보통)</v>
+      </c>
+      <c r="G392" t="s">
+        <v>988</v>
+      </c>
+      <c r="H392" t="s">
+        <v>988</v>
+      </c>
+      <c r="I392" t="s">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="393" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A393" t="s">
         <v>4</v>
       </c>
@@ -19072,10 +19407,19 @@
       </c>
       <c r="F393" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="394" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 크게, 입 크게, 고개 돌림 없음)</v>
+      </c>
+      <c r="G393" t="s">
+        <v>991</v>
+      </c>
+      <c r="H393" t="s">
+        <v>991</v>
+      </c>
+      <c r="I393" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="394" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A394" t="s">
         <v>4</v>
       </c>
@@ -19090,10 +19434,19 @@
       </c>
       <c r="F394" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="395" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 보통, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G394" t="s">
+        <v>988</v>
+      </c>
+      <c r="H394" t="s">
+        <v>988</v>
+      </c>
+      <c r="I394" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="395" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A395" t="s">
         <v>4</v>
       </c>
@@ -19108,10 +19461,19 @@
       </c>
       <c r="F395" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="396" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 보통, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G395" t="s">
+        <v>988</v>
+      </c>
+      <c r="H395" t="s">
+        <v>988</v>
+      </c>
+      <c r="I395" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="396" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A396" t="s">
         <v>4</v>
       </c>
@@ -19129,10 +19491,19 @@
       </c>
       <c r="F396" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="397" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 아주 크게, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G396" t="s">
+        <v>992</v>
+      </c>
+      <c r="H396" t="s">
+        <v>988</v>
+      </c>
+      <c r="I396" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="397" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A397" t="s">
         <v>4</v>
       </c>
@@ -19147,10 +19518,19 @@
       </c>
       <c r="F397" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="398" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 보통, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G397" t="s">
+        <v>988</v>
+      </c>
+      <c r="H397" t="s">
+        <v>988</v>
+      </c>
+      <c r="I397" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="398" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A398" t="s">
         <v>4</v>
       </c>
@@ -19165,10 +19545,19 @@
       </c>
       <c r="F398" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="399" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 보통, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G398" t="s">
+        <v>988</v>
+      </c>
+      <c r="H398" t="s">
+        <v>988</v>
+      </c>
+      <c r="I398" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="399" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A399" t="s">
         <v>4</v>
       </c>
@@ -19186,10 +19575,19 @@
       </c>
       <c r="F399" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="400" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 보통, 입 크게, 고개 돌림 없음)</v>
+      </c>
+      <c r="G399" t="s">
+        <v>988</v>
+      </c>
+      <c r="H399" t="s">
+        <v>991</v>
+      </c>
+      <c r="I399" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="400" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A400" t="s">
         <v>4</v>
       </c>
@@ -19207,10 +19605,19 @@
       </c>
       <c r="F400" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="401" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 보통, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G400" t="s">
+        <v>988</v>
+      </c>
+      <c r="H400" t="s">
+        <v>988</v>
+      </c>
+      <c r="I400" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="401" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A401" t="s">
         <v>4</v>
       </c>
@@ -19228,10 +19635,19 @@
       </c>
       <c r="F401" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="402" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 보통, 입 크게, 고개 돌림 없음)</v>
+      </c>
+      <c r="G401" t="s">
+        <v>988</v>
+      </c>
+      <c r="H401" t="s">
+        <v>991</v>
+      </c>
+      <c r="I401" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="402" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A402" t="s">
         <v>4</v>
       </c>
@@ -19246,10 +19662,19 @@
       </c>
       <c r="F402" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="403" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 크게, 입 크게, 고개 돌림 없음)</v>
+      </c>
+      <c r="G402" t="s">
+        <v>991</v>
+      </c>
+      <c r="H402" t="s">
+        <v>991</v>
+      </c>
+      <c r="I402" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="403" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A403" t="s">
         <v>4</v>
       </c>
@@ -19267,10 +19692,19 @@
       </c>
       <c r="F403" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="404" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 크게, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G403" t="s">
+        <v>991</v>
+      </c>
+      <c r="H403" t="s">
+        <v>988</v>
+      </c>
+      <c r="I403" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="404" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A404" t="s">
         <v>4</v>
       </c>
@@ -19288,10 +19722,19 @@
       </c>
       <c r="F404" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="405" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 크게, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G404" t="s">
+        <v>991</v>
+      </c>
+      <c r="H404" t="s">
+        <v>988</v>
+      </c>
+      <c r="I404" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="405" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A405" t="s">
         <v>4</v>
       </c>
@@ -19309,10 +19752,19 @@
       </c>
       <c r="F405" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="406" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 보통, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G405" t="s">
+        <v>988</v>
+      </c>
+      <c r="H405" t="s">
+        <v>988</v>
+      </c>
+      <c r="I405" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="406" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A406" t="s">
         <v>4</v>
       </c>
@@ -19330,10 +19782,19 @@
       </c>
       <c r="F406" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="407" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 보통, 입 크게, 고개 돌림 없음)</v>
+      </c>
+      <c r="G406" t="s">
+        <v>988</v>
+      </c>
+      <c r="H406" t="s">
+        <v>991</v>
+      </c>
+      <c r="I406" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="407" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A407" t="s">
         <v>4</v>
       </c>
@@ -19351,10 +19812,19 @@
       </c>
       <c r="F407" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="408" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 보통, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G407" t="s">
+        <v>988</v>
+      </c>
+      <c r="H407" t="s">
+        <v>988</v>
+      </c>
+      <c r="I407" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="408" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A408" t="s">
         <v>4</v>
       </c>
@@ -19372,10 +19842,19 @@
       </c>
       <c r="F408" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="409" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 크게, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G408" t="s">
+        <v>991</v>
+      </c>
+      <c r="H408" t="s">
+        <v>988</v>
+      </c>
+      <c r="I408" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="409" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A409" t="s">
         <v>4</v>
       </c>
@@ -19393,10 +19872,19 @@
       </c>
       <c r="F409" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="410" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 크게, 입 크게, 고개 돌림 없음)</v>
+      </c>
+      <c r="G409" t="s">
+        <v>991</v>
+      </c>
+      <c r="H409" t="s">
+        <v>991</v>
+      </c>
+      <c r="I409" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="410" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A410" t="s">
         <v>4</v>
       </c>
@@ -19414,10 +19902,19 @@
       </c>
       <c r="F410" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="411" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 보통, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G410" t="s">
+        <v>988</v>
+      </c>
+      <c r="H410" t="s">
+        <v>988</v>
+      </c>
+      <c r="I410" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="411" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A411" t="s">
         <v>4</v>
       </c>
@@ -19432,10 +19929,19 @@
       </c>
       <c r="F411" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="412" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 보통, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G411" t="s">
+        <v>988</v>
+      </c>
+      <c r="H411" t="s">
+        <v>988</v>
+      </c>
+      <c r="I411" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="412" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A412" t="s">
         <v>4</v>
       </c>
@@ -19450,10 +19956,19 @@
       </c>
       <c r="F412" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="413" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 보통, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G412" t="s">
+        <v>988</v>
+      </c>
+      <c r="H412" t="s">
+        <v>988</v>
+      </c>
+      <c r="I412" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="413" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A413" t="s">
         <v>4</v>
       </c>
@@ -19471,10 +19986,19 @@
       </c>
       <c r="F413" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="414" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 보통, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G413" t="s">
+        <v>988</v>
+      </c>
+      <c r="H413" t="s">
+        <v>988</v>
+      </c>
+      <c r="I413" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="414" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A414" t="s">
         <v>4</v>
       </c>
@@ -19492,10 +20016,19 @@
       </c>
       <c r="F414" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="415" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 보통, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G414" t="s">
+        <v>988</v>
+      </c>
+      <c r="H414" t="s">
+        <v>988</v>
+      </c>
+      <c r="I414" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="415" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A415" t="s">
         <v>4</v>
       </c>
@@ -19513,10 +20046,19 @@
       </c>
       <c r="F415" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="416" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 보통, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G415" t="s">
+        <v>988</v>
+      </c>
+      <c r="H415" t="s">
+        <v>988</v>
+      </c>
+      <c r="I415" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="416" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A416" t="s">
         <v>4</v>
       </c>
@@ -19534,10 +20076,19 @@
       </c>
       <c r="F416" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="417" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 보통, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G416" t="s">
+        <v>988</v>
+      </c>
+      <c r="H416" t="s">
+        <v>988</v>
+      </c>
+      <c r="I416" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="417" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A417" t="s">
         <v>4</v>
       </c>
@@ -19555,10 +20106,19 @@
       </c>
       <c r="F417" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="418" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 보통, 입 크게, 고개 돌림 없음)</v>
+      </c>
+      <c r="G417" t="s">
+        <v>988</v>
+      </c>
+      <c r="H417" t="s">
+        <v>991</v>
+      </c>
+      <c r="I417" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="418" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A418" t="s">
         <v>4</v>
       </c>
@@ -19576,10 +20136,19 @@
       </c>
       <c r="F418" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="419" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 보통, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G418" t="s">
+        <v>988</v>
+      </c>
+      <c r="H418" t="s">
+        <v>988</v>
+      </c>
+      <c r="I418" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="419" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A419" t="s">
         <v>4</v>
       </c>
@@ -19594,10 +20163,19 @@
       </c>
       <c r="F419" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="420" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 보통, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G419" t="s">
+        <v>988</v>
+      </c>
+      <c r="H419" t="s">
+        <v>988</v>
+      </c>
+      <c r="I419" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="420" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A420" t="s">
         <v>4</v>
       </c>
@@ -19612,10 +20190,19 @@
       </c>
       <c r="F420" t="str">
         <f t="shared" si="6"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="421" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 크게, 입 아주 크게, 고개 돌림 없음)</v>
+      </c>
+      <c r="G420" t="s">
+        <v>991</v>
+      </c>
+      <c r="H420" t="s">
+        <v>992</v>
+      </c>
+      <c r="I420" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="421" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A421" t="s">
         <v>4</v>
       </c>
@@ -19630,10 +20217,19 @@
       </c>
       <c r="F421" t="str">
         <f t="shared" ref="F421:F426" si="7">"(눈 "&amp;G421&amp;", 입 "&amp;H421&amp;", 고개 돌림 "&amp;I421&amp;")"</f>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="422" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 크게, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G421" t="s">
+        <v>991</v>
+      </c>
+      <c r="H421" t="s">
+        <v>988</v>
+      </c>
+      <c r="I421" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="422" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A422" t="s">
         <v>4</v>
       </c>
@@ -19648,10 +20244,19 @@
       </c>
       <c r="F422" t="str">
         <f t="shared" si="7"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="423" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 크게, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G422" t="s">
+        <v>991</v>
+      </c>
+      <c r="H422" t="s">
+        <v>988</v>
+      </c>
+      <c r="I422" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="423" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A423" t="s">
         <v>4</v>
       </c>
@@ -19666,10 +20271,19 @@
       </c>
       <c r="F423" t="str">
         <f t="shared" si="7"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="424" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 보통, 입 아주 크게, 고개 돌림 없음)</v>
+      </c>
+      <c r="G423" t="s">
+        <v>988</v>
+      </c>
+      <c r="H423" t="s">
+        <v>992</v>
+      </c>
+      <c r="I423" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="424" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A424" t="s">
         <v>4</v>
       </c>
@@ -19684,10 +20298,19 @@
       </c>
       <c r="F424" t="str">
         <f t="shared" si="7"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="425" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 크게, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G424" t="s">
+        <v>991</v>
+      </c>
+      <c r="H424" t="s">
+        <v>988</v>
+      </c>
+      <c r="I424" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="425" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A425" t="s">
         <v>4</v>
       </c>
@@ -19705,10 +20328,19 @@
       </c>
       <c r="F425" t="str">
         <f t="shared" si="7"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="426" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 보통, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G425" t="s">
+        <v>988</v>
+      </c>
+      <c r="H425" t="s">
+        <v>988</v>
+      </c>
+      <c r="I425" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="426" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A426" t="s">
         <v>4</v>
       </c>
@@ -19726,10 +20358,19 @@
       </c>
       <c r="F426" t="str">
         <f t="shared" si="7"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="427" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 보통, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G426" t="s">
+        <v>988</v>
+      </c>
+      <c r="H426" t="s">
+        <v>988</v>
+      </c>
+      <c r="I426" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="427" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A427" t="s">
         <v>4</v>
       </c>
@@ -19747,10 +20388,19 @@
       </c>
       <c r="F427" t="str">
         <f t="shared" ref="F427:F444" si="8">"(눈 "&amp;G427&amp;", 입 "&amp;H427&amp;", 고개 돌림 "&amp;I427&amp;")"</f>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="428" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 보통, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G427" t="s">
+        <v>988</v>
+      </c>
+      <c r="H427" t="s">
+        <v>988</v>
+      </c>
+      <c r="I427" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="428" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A428" t="s">
         <v>4</v>
       </c>
@@ -19765,10 +20415,19 @@
       </c>
       <c r="F428" t="str">
         <f t="shared" si="8"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="429" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 보통, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G428" t="s">
+        <v>988</v>
+      </c>
+      <c r="H428" t="s">
+        <v>988</v>
+      </c>
+      <c r="I428" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="429" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A429" t="s">
         <v>4</v>
       </c>
@@ -19783,10 +20442,19 @@
       </c>
       <c r="F429" t="str">
         <f t="shared" si="8"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="430" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 크게, 입 크게, 고개 돌림 없음)</v>
+      </c>
+      <c r="G429" t="s">
+        <v>991</v>
+      </c>
+      <c r="H429" t="s">
+        <v>991</v>
+      </c>
+      <c r="I429" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="430" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A430" t="s">
         <v>4</v>
       </c>
@@ -19801,10 +20469,19 @@
       </c>
       <c r="F430" t="str">
         <f t="shared" si="8"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="431" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 보통, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G430" t="s">
+        <v>988</v>
+      </c>
+      <c r="H430" t="s">
+        <v>988</v>
+      </c>
+      <c r="I430" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="431" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A431" t="s">
         <v>4</v>
       </c>
@@ -19822,10 +20499,19 @@
       </c>
       <c r="F431" t="str">
         <f t="shared" si="8"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="432" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 크게, 입 크게, 고개 돌림 없음)</v>
+      </c>
+      <c r="G431" t="s">
+        <v>991</v>
+      </c>
+      <c r="H431" t="s">
+        <v>991</v>
+      </c>
+      <c r="I431" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="432" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A432" t="s">
         <v>4</v>
       </c>
@@ -19840,10 +20526,19 @@
       </c>
       <c r="F432" t="str">
         <f t="shared" si="8"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="433" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 작게, 입 보통, 고개 돌림 보통)</v>
+      </c>
+      <c r="G432" t="s">
+        <v>987</v>
+      </c>
+      <c r="H432" t="s">
+        <v>988</v>
+      </c>
+      <c r="I432" t="s">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="433" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A433" t="s">
         <v>4</v>
       </c>
@@ -19858,10 +20553,19 @@
       </c>
       <c r="F433" t="str">
         <f t="shared" si="8"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="434" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 크게, 입 크게, 고개 돌림 없음)</v>
+      </c>
+      <c r="G433" t="s">
+        <v>991</v>
+      </c>
+      <c r="H433" t="s">
+        <v>991</v>
+      </c>
+      <c r="I433" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="434" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A434" t="s">
         <v>4</v>
       </c>
@@ -19879,10 +20583,19 @@
       </c>
       <c r="F434" t="str">
         <f t="shared" si="8"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="435" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 작게, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G434" t="s">
+        <v>987</v>
+      </c>
+      <c r="H434" t="s">
+        <v>988</v>
+      </c>
+      <c r="I434" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="435" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A435" t="s">
         <v>4</v>
       </c>
@@ -19900,10 +20613,19 @@
       </c>
       <c r="F435" t="str">
         <f t="shared" si="8"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="436" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 작게, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G435" t="s">
+        <v>987</v>
+      </c>
+      <c r="H435" t="s">
+        <v>988</v>
+      </c>
+      <c r="I435" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="436" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A436" t="s">
         <v>4</v>
       </c>
@@ -19918,10 +20640,19 @@
       </c>
       <c r="F436" t="str">
         <f t="shared" si="8"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="437" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 보통, 입 크게, 고개 돌림 없음)</v>
+      </c>
+      <c r="G436" t="s">
+        <v>988</v>
+      </c>
+      <c r="H436" t="s">
+        <v>991</v>
+      </c>
+      <c r="I436" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="437" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A437" t="s">
         <v>4</v>
       </c>
@@ -19939,10 +20670,19 @@
       </c>
       <c r="F437" t="str">
         <f t="shared" si="8"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="438" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 크게, 입 크게, 고개 돌림 없음)</v>
+      </c>
+      <c r="G437" t="s">
+        <v>991</v>
+      </c>
+      <c r="H437" t="s">
+        <v>991</v>
+      </c>
+      <c r="I437" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="438" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A438" t="s">
         <v>4</v>
       </c>
@@ -19960,10 +20700,19 @@
       </c>
       <c r="F438" t="str">
         <f t="shared" si="8"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="439" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 보통, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G438" t="s">
+        <v>988</v>
+      </c>
+      <c r="H438" t="s">
+        <v>988</v>
+      </c>
+      <c r="I438" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="439" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A439" t="s">
         <v>4</v>
       </c>
@@ -19981,10 +20730,19 @@
       </c>
       <c r="F439" t="str">
         <f t="shared" si="8"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="440" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 크게, 입 크게, 고개 돌림 없음)</v>
+      </c>
+      <c r="G439" t="s">
+        <v>991</v>
+      </c>
+      <c r="H439" t="s">
+        <v>991</v>
+      </c>
+      <c r="I439" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="440" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A440" t="s">
         <v>4</v>
       </c>
@@ -20002,10 +20760,19 @@
       </c>
       <c r="F440" t="str">
         <f t="shared" si="8"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="441" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 크게, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G440" t="s">
+        <v>991</v>
+      </c>
+      <c r="H440" t="s">
+        <v>988</v>
+      </c>
+      <c r="I440" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="441" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A441" t="s">
         <v>4</v>
       </c>
@@ -20023,10 +20790,19 @@
       </c>
       <c r="F441" t="str">
         <f t="shared" si="8"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="442" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 크게, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G441" t="s">
+        <v>991</v>
+      </c>
+      <c r="H441" t="s">
+        <v>988</v>
+      </c>
+      <c r="I441" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="442" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A442" t="s">
         <v>4</v>
       </c>
@@ -20041,10 +20817,19 @@
       </c>
       <c r="F442" t="str">
         <f t="shared" si="8"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="443" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 작게, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G442" t="s">
+        <v>987</v>
+      </c>
+      <c r="H442" t="s">
+        <v>988</v>
+      </c>
+      <c r="I442" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="443" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A443" t="s">
         <v>4</v>
       </c>
@@ -20059,10 +20844,19 @@
       </c>
       <c r="F443" t="str">
         <f t="shared" si="8"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="444" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 보통, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G443" t="s">
+        <v>988</v>
+      </c>
+      <c r="H443" t="s">
+        <v>988</v>
+      </c>
+      <c r="I443" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="444" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A444" t="s">
         <v>4</v>
       </c>
@@ -20080,10 +20874,19 @@
       </c>
       <c r="F444" t="str">
         <f t="shared" si="8"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="445" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 크게, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G444" t="s">
+        <v>991</v>
+      </c>
+      <c r="H444" t="s">
+        <v>988</v>
+      </c>
+      <c r="I444" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="445" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A445" t="s">
         <v>4</v>
       </c>
@@ -20098,10 +20901,19 @@
       </c>
       <c r="F445" t="str">
         <f t="shared" ref="F445:F449" si="9">"(눈 "&amp;G445&amp;", 입 "&amp;H445&amp;", 고개 돌림 "&amp;I445&amp;")"</f>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="446" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 보통, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G445" t="s">
+        <v>988</v>
+      </c>
+      <c r="H445" t="s">
+        <v>988</v>
+      </c>
+      <c r="I445" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="446" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A446" t="s">
         <v>4</v>
       </c>
@@ -20116,10 +20928,19 @@
       </c>
       <c r="F446" t="str">
         <f t="shared" si="9"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="447" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 보통, 입 크게, 고개 돌림 없음)</v>
+      </c>
+      <c r="G446" t="s">
+        <v>988</v>
+      </c>
+      <c r="H446" t="s">
+        <v>991</v>
+      </c>
+      <c r="I446" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="447" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A447" t="s">
         <v>4</v>
       </c>
@@ -20134,10 +20955,19 @@
       </c>
       <c r="F447" t="str">
         <f t="shared" si="9"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="448" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 크게, 입 크게, 고개 돌림 없음)</v>
+      </c>
+      <c r="G447" t="s">
+        <v>991</v>
+      </c>
+      <c r="H447" t="s">
+        <v>991</v>
+      </c>
+      <c r="I447" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="448" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A448" t="s">
         <v>4</v>
       </c>
@@ -20155,10 +20985,19 @@
       </c>
       <c r="F448" t="str">
         <f t="shared" si="9"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="449" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 보통, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G448" t="s">
+        <v>988</v>
+      </c>
+      <c r="H448" t="s">
+        <v>988</v>
+      </c>
+      <c r="I448" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="449" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A449" t="s">
         <v>4</v>
       </c>
@@ -20173,10 +21012,19 @@
       </c>
       <c r="F449" t="str">
         <f t="shared" si="9"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="450" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 보통, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G449" t="s">
+        <v>988</v>
+      </c>
+      <c r="H449" t="s">
+        <v>988</v>
+      </c>
+      <c r="I449" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="450" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A450" t="s">
         <v>4</v>
       </c>
@@ -20191,10 +21039,19 @@
       </c>
       <c r="F450" t="str">
         <f t="shared" ref="F450:F457" si="10">"(눈 "&amp;G450&amp;", 입 "&amp;H450&amp;", 고개 돌림 "&amp;I450&amp;")"</f>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="451" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 작게, 입 보통, 고개 돌림 보통)</v>
+      </c>
+      <c r="G450" t="s">
+        <v>987</v>
+      </c>
+      <c r="H450" t="s">
+        <v>988</v>
+      </c>
+      <c r="I450" t="s">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="451" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A451" t="s">
         <v>4</v>
       </c>
@@ -20212,10 +21069,19 @@
       </c>
       <c r="F451" t="str">
         <f t="shared" si="10"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="452" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 보통, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G451" t="s">
+        <v>988</v>
+      </c>
+      <c r="H451" t="s">
+        <v>988</v>
+      </c>
+      <c r="I451" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="452" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A452" t="s">
         <v>4</v>
       </c>
@@ -20230,10 +21096,19 @@
       </c>
       <c r="F452" t="str">
         <f t="shared" si="10"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="453" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 보통, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G452" t="s">
+        <v>988</v>
+      </c>
+      <c r="H452" t="s">
+        <v>988</v>
+      </c>
+      <c r="I452" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="453" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A453" t="s">
         <v>4</v>
       </c>
@@ -20251,10 +21126,19 @@
       </c>
       <c r="F453" t="str">
         <f t="shared" si="10"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="454" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 크게, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G453" t="s">
+        <v>991</v>
+      </c>
+      <c r="H453" t="s">
+        <v>988</v>
+      </c>
+      <c r="I453" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="454" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A454" t="s">
         <v>4</v>
       </c>
@@ -20272,10 +21156,19 @@
       </c>
       <c r="F454" t="str">
         <f t="shared" si="10"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="455" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 보통, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G454" t="s">
+        <v>988</v>
+      </c>
+      <c r="H454" t="s">
+        <v>988</v>
+      </c>
+      <c r="I454" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="455" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A455" t="s">
         <v>4</v>
       </c>
@@ -20290,10 +21183,19 @@
       </c>
       <c r="F455" t="str">
         <f t="shared" si="10"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="456" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 보통, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G455" t="s">
+        <v>988</v>
+      </c>
+      <c r="H455" t="s">
+        <v>988</v>
+      </c>
+      <c r="I455" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="456" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A456" t="s">
         <v>4</v>
       </c>
@@ -20311,10 +21213,19 @@
       </c>
       <c r="F456" t="str">
         <f t="shared" si="10"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="457" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 보통, 입 보통, 고개 돌림 없음)</v>
+      </c>
+      <c r="G456" t="s">
+        <v>988</v>
+      </c>
+      <c r="H456" t="s">
+        <v>988</v>
+      </c>
+      <c r="I456" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="457" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A457" t="s">
         <v>4</v>
       </c>
@@ -20332,10 +21243,19 @@
       </c>
       <c r="F457" t="str">
         <f t="shared" si="10"/>
-        <v>(눈 , 입 , 고개 돌림 )</v>
-      </c>
-    </row>
-    <row r="458" spans="1:6" x14ac:dyDescent="0.4">
+        <v>(눈 크게, 입 크게, 고개 돌림 없음)</v>
+      </c>
+      <c r="G457" t="s">
+        <v>991</v>
+      </c>
+      <c r="H457" t="s">
+        <v>991</v>
+      </c>
+      <c r="I457" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="458" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A458" t="s">
         <v>433</v>
       </c>
@@ -20343,7 +21263,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="459" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="459" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A459" t="s">
         <v>433</v>
       </c>
@@ -20351,7 +21271,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="460" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="460" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A460" t="s">
         <v>433</v>
       </c>
@@ -20359,7 +21279,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="461" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="461" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A461" t="s">
         <v>433</v>
       </c>
@@ -20367,7 +21287,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="462" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="462" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A462" t="s">
         <v>433</v>
       </c>
@@ -20375,7 +21295,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="463" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="463" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A463" t="s">
         <v>433</v>
       </c>
@@ -20383,7 +21303,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="464" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="464" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A464" t="s">
         <v>433</v>
       </c>

</xml_diff>